<commit_message>
Latest generated outputs 2025-09-19
</commit_message>
<xml_diff>
--- a/generated/spreadsheet/full-planning-permission-full.xlsx
+++ b/generated/spreadsheet/full-planning-permission-full.xlsx
@@ -4244,7 +4244,7 @@
       <c r="B120" s="2" t="n"/>
       <c r="C120" s="2" t="inlineStr">
         <is>
-          <t>Additional material information</t>
+          <t>Providing additional material information</t>
         </is>
       </c>
       <c r="D120" s="2" t="inlineStr"/>
@@ -4252,12 +4252,12 @@
       <c r="F120" s="2" t="inlineStr"/>
       <c r="G120" s="2" t="inlineStr">
         <is>
-          <t>Additional context or details about the materials to be used in the development</t>
+          <t>Is the applicant providing additional materials information on submitted plan(s)/drawing(s)/design and access statement?</t>
         </is>
       </c>
       <c r="H120" s="2" t="inlineStr">
         <is>
-          <t>string</t>
+          <t>boolean</t>
         </is>
       </c>
       <c r="I120" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Latest generated outputs 2025-10-27
</commit_message>
<xml_diff>
--- a/generated/spreadsheet/full-planning-permission-full.xlsx
+++ b/generated/spreadsheet/full-planning-permission-full.xlsx
@@ -427,7 +427,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I216"/>
+  <dimension ref="A1:I217"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4559,14 +4559,14 @@
       </c>
       <c r="D130" s="2" t="inlineStr">
         <is>
-          <t>Use class</t>
+          <t>Use class for accommodation</t>
         </is>
       </c>
       <c r="E130" s="2" t="inlineStr"/>
       <c r="F130" s="2" t="inlineStr"/>
       <c r="G130" s="2" t="inlineStr">
         <is>
-          <t>Type of non-residential use class</t>
+          <t>Type of non-residential use class referring to accommodation uses</t>
         </is>
       </c>
       <c r="H130" s="2" t="inlineStr">
@@ -4590,24 +4590,24 @@
       </c>
       <c r="D131" s="2" t="inlineStr">
         <is>
-          <t>Existing rooms lost</t>
+          <t>Use other</t>
         </is>
       </c>
       <c r="E131" s="2" t="inlineStr"/>
       <c r="F131" s="2" t="inlineStr"/>
       <c r="G131" s="2" t="inlineStr">
         <is>
-          <t>Existing rooms to be lost by change of use</t>
+          <t>Specify use if use is "other"</t>
         </is>
       </c>
       <c r="H131" s="2" t="inlineStr">
         <is>
-          <t>number</t>
+          <t>string</t>
         </is>
       </c>
       <c r="I131" s="2" t="inlineStr">
         <is>
-          <t>MUST</t>
+          <t>MAY</t>
         </is>
       </c>
     </row>
@@ -4621,14 +4621,14 @@
       </c>
       <c r="D132" s="2" t="inlineStr">
         <is>
-          <t>Total rooms proposed</t>
+          <t>Existing rooms lost</t>
         </is>
       </c>
       <c r="E132" s="2" t="inlineStr"/>
       <c r="F132" s="2" t="inlineStr"/>
       <c r="G132" s="2" t="inlineStr">
         <is>
-          <t>Total rooms proposed (including change of use)</t>
+          <t>Existing rooms to be lost by change of use</t>
         </is>
       </c>
       <c r="H132" s="2" t="inlineStr">
@@ -4652,14 +4652,14 @@
       </c>
       <c r="D133" s="2" t="inlineStr">
         <is>
-          <t>Net additional rooms</t>
+          <t>Total rooms proposed</t>
         </is>
       </c>
       <c r="E133" s="2" t="inlineStr"/>
       <c r="F133" s="2" t="inlineStr"/>
       <c r="G133" s="2" t="inlineStr">
         <is>
-          <t>Net additional rooms following development</t>
+          <t>Total rooms proposed (including change of use)</t>
         </is>
       </c>
       <c r="H133" s="2" t="inlineStr">
@@ -4674,32 +4674,28 @@
       </c>
     </row>
     <row r="134">
-      <c r="A134" s="2" t="inlineStr">
-        <is>
-          <t>Ownership certificates and agricultural land declaration</t>
-        </is>
-      </c>
-      <c r="B134" s="2" t="inlineStr">
-        <is>
-          <t>Who will be affected by the proposal and whether they have been notified, such as agricultural tenants</t>
-        </is>
-      </c>
+      <c r="A134" s="2" t="n"/>
+      <c r="B134" s="2" t="n"/>
       <c r="C134" s="2" t="inlineStr">
         <is>
-          <t>Sole owner</t>
-        </is>
-      </c>
-      <c r="D134" s="2" t="inlineStr"/>
+          <t>Room details[]</t>
+        </is>
+      </c>
+      <c r="D134" s="2" t="inlineStr">
+        <is>
+          <t>Net additional rooms</t>
+        </is>
+      </c>
       <c r="E134" s="2" t="inlineStr"/>
       <c r="F134" s="2" t="inlineStr"/>
       <c r="G134" s="2" t="inlineStr">
         <is>
-          <t>Is the applicant the sole owner of the land?</t>
+          <t>Net additional rooms following development</t>
         </is>
       </c>
       <c r="H134" s="2" t="inlineStr">
         <is>
-          <t>boolean</t>
+          <t>number</t>
         </is>
       </c>
       <c r="I134" s="2" t="inlineStr">
@@ -4709,11 +4705,19 @@
       </c>
     </row>
     <row r="135">
-      <c r="A135" s="2" t="n"/>
-      <c r="B135" s="2" t="n"/>
+      <c r="A135" s="2" t="inlineStr">
+        <is>
+          <t>Ownership certificates and agricultural land declaration</t>
+        </is>
+      </c>
+      <c r="B135" s="2" t="inlineStr">
+        <is>
+          <t>Who will be affected by the proposal and whether they have been notified, such as agricultural tenants</t>
+        </is>
+      </c>
       <c r="C135" s="2" t="inlineStr">
         <is>
-          <t>Agricultural tenants</t>
+          <t>Sole owner</t>
         </is>
       </c>
       <c r="D135" s="2" t="inlineStr"/>
@@ -4721,7 +4725,7 @@
       <c r="F135" s="2" t="inlineStr"/>
       <c r="G135" s="2" t="inlineStr">
         <is>
-          <t>Are there any agricultural tenants on the land?</t>
+          <t>Is the applicant the sole owner of the land?</t>
         </is>
       </c>
       <c r="H135" s="2" t="inlineStr">
@@ -4740,33 +4744,25 @@
       <c r="B136" s="2" t="n"/>
       <c r="C136" s="2" t="inlineStr">
         <is>
-          <t>Owners and tenants[]</t>
-        </is>
-      </c>
-      <c r="D136" s="2" t="inlineStr">
-        <is>
-          <t>Person</t>
-        </is>
-      </c>
-      <c r="E136" s="2" t="inlineStr">
-        <is>
-          <t>Title</t>
-        </is>
-      </c>
+          <t>Agricultural tenants</t>
+        </is>
+      </c>
+      <c r="D136" s="2" t="inlineStr"/>
+      <c r="E136" s="2" t="inlineStr"/>
       <c r="F136" s="2" t="inlineStr"/>
       <c r="G136" s="2" t="inlineStr">
         <is>
-          <t>The title of the individual</t>
+          <t>Are there any agricultural tenants on the land?</t>
         </is>
       </c>
       <c r="H136" s="2" t="inlineStr">
         <is>
-          <t>string</t>
+          <t>boolean</t>
         </is>
       </c>
       <c r="I136" s="2" t="inlineStr">
         <is>
-          <t>MAY</t>
+          <t>MUST</t>
         </is>
       </c>
     </row>
@@ -4785,13 +4781,13 @@
       </c>
       <c r="E137" s="2" t="inlineStr">
         <is>
-          <t>First Name</t>
+          <t>Title</t>
         </is>
       </c>
       <c r="F137" s="2" t="inlineStr"/>
       <c r="G137" s="2" t="inlineStr">
         <is>
-          <t>The first name of the individual</t>
+          <t>The title of the individual</t>
         </is>
       </c>
       <c r="H137" s="2" t="inlineStr">
@@ -4801,7 +4797,7 @@
       </c>
       <c r="I137" s="2" t="inlineStr">
         <is>
-          <t>MUST</t>
+          <t>MAY</t>
         </is>
       </c>
     </row>
@@ -4820,13 +4816,13 @@
       </c>
       <c r="E138" s="2" t="inlineStr">
         <is>
-          <t>Last Name</t>
+          <t>First Name</t>
         </is>
       </c>
       <c r="F138" s="2" t="inlineStr"/>
       <c r="G138" s="2" t="inlineStr">
         <is>
-          <t>The last name of the individual</t>
+          <t>The first name of the individual</t>
         </is>
       </c>
       <c r="H138" s="2" t="inlineStr">
@@ -4855,13 +4851,13 @@
       </c>
       <c r="E139" s="2" t="inlineStr">
         <is>
-          <t>Address Text</t>
+          <t>Last Name</t>
         </is>
       </c>
       <c r="F139" s="2" t="inlineStr"/>
       <c r="G139" s="2" t="inlineStr">
         <is>
-          <t>Flexible field for capturing addresses</t>
+          <t>The last name of the individual</t>
         </is>
       </c>
       <c r="H139" s="2" t="inlineStr">
@@ -4890,13 +4886,13 @@
       </c>
       <c r="E140" s="2" t="inlineStr">
         <is>
-          <t>Postcode</t>
+          <t>Address Text</t>
         </is>
       </c>
       <c r="F140" s="2" t="inlineStr"/>
       <c r="G140" s="2" t="inlineStr">
         <is>
-          <t>The postal code</t>
+          <t>Flexible field for capturing addresses</t>
         </is>
       </c>
       <c r="H140" s="2" t="inlineStr">
@@ -4906,7 +4902,7 @@
       </c>
       <c r="I140" s="2" t="inlineStr">
         <is>
-          <t>MAY</t>
+          <t>MUST</t>
         </is>
       </c>
     </row>
@@ -4920,19 +4916,23 @@
       </c>
       <c r="D141" s="2" t="inlineStr">
         <is>
-          <t>Notice date</t>
-        </is>
-      </c>
-      <c r="E141" s="2" t="inlineStr"/>
+          <t>Person</t>
+        </is>
+      </c>
+      <c r="E141" s="2" t="inlineStr">
+        <is>
+          <t>Postcode</t>
+        </is>
+      </c>
       <c r="F141" s="2" t="inlineStr"/>
       <c r="G141" s="2" t="inlineStr">
         <is>
-          <t>Date when notice was served</t>
+          <t>The postal code</t>
         </is>
       </c>
       <c r="H141" s="2" t="inlineStr">
         <is>
-          <t>date</t>
+          <t>string</t>
         </is>
       </c>
       <c r="I141" s="2" t="inlineStr">
@@ -4946,20 +4946,24 @@
       <c r="B142" s="2" t="n"/>
       <c r="C142" s="2" t="inlineStr">
         <is>
-          <t>Steps taken</t>
-        </is>
-      </c>
-      <c r="D142" s="2" t="inlineStr"/>
+          <t>Owners and tenants[]</t>
+        </is>
+      </c>
+      <c r="D142" s="2" t="inlineStr">
+        <is>
+          <t>Notice date</t>
+        </is>
+      </c>
       <c r="E142" s="2" t="inlineStr"/>
       <c r="F142" s="2" t="inlineStr"/>
       <c r="G142" s="2" t="inlineStr">
         <is>
-          <t>Description of steps taken to identify unknown owners or tenants</t>
+          <t>Date when notice was served</t>
         </is>
       </c>
       <c r="H142" s="2" t="inlineStr">
         <is>
-          <t>string</t>
+          <t>date</t>
         </is>
       </c>
       <c r="I142" s="2" t="inlineStr">
@@ -4973,19 +4977,15 @@
       <c r="B143" s="2" t="n"/>
       <c r="C143" s="2" t="inlineStr">
         <is>
-          <t>Newspaper notices[]</t>
-        </is>
-      </c>
-      <c r="D143" s="2" t="inlineStr">
-        <is>
-          <t>Newspaper name</t>
-        </is>
-      </c>
+          <t>Steps taken</t>
+        </is>
+      </c>
+      <c r="D143" s="2" t="inlineStr"/>
       <c r="E143" s="2" t="inlineStr"/>
       <c r="F143" s="2" t="inlineStr"/>
       <c r="G143" s="2" t="inlineStr">
         <is>
-          <t>Name of the newspaper where notice was published</t>
+          <t>Description of steps taken to identify unknown owners or tenants</t>
         </is>
       </c>
       <c r="H143" s="2" t="inlineStr">
@@ -4995,7 +4995,7 @@
       </c>
       <c r="I143" s="2" t="inlineStr">
         <is>
-          <t>MUST</t>
+          <t>MAY</t>
         </is>
       </c>
     </row>
@@ -5009,19 +5009,19 @@
       </c>
       <c r="D144" s="2" t="inlineStr">
         <is>
-          <t>Publication date</t>
+          <t>Newspaper name</t>
         </is>
       </c>
       <c r="E144" s="2" t="inlineStr"/>
       <c r="F144" s="2" t="inlineStr"/>
       <c r="G144" s="2" t="inlineStr">
         <is>
-          <t>Date when the notice was published</t>
+          <t>Name of the newspaper where notice was published</t>
         </is>
       </c>
       <c r="H144" s="2" t="inlineStr">
         <is>
-          <t>date</t>
+          <t>string</t>
         </is>
       </c>
       <c r="I144" s="2" t="inlineStr">
@@ -5035,25 +5035,29 @@
       <c r="B145" s="2" t="n"/>
       <c r="C145" s="2" t="inlineStr">
         <is>
-          <t>Ownership certificate type</t>
-        </is>
-      </c>
-      <c r="D145" s="2" t="inlineStr"/>
+          <t>Newspaper notices[]</t>
+        </is>
+      </c>
+      <c r="D145" s="2" t="inlineStr">
+        <is>
+          <t>Publication date</t>
+        </is>
+      </c>
       <c r="E145" s="2" t="inlineStr"/>
       <c r="F145" s="2" t="inlineStr"/>
       <c r="G145" s="2" t="inlineStr">
         <is>
-          <t>The type of ownership certificate based on ownership and tenancy status</t>
+          <t>Date when the notice was published</t>
         </is>
       </c>
       <c r="H145" s="2" t="inlineStr">
         <is>
-          <t>enum</t>
+          <t>date</t>
         </is>
       </c>
       <c r="I145" s="2" t="inlineStr">
         <is>
-          <t>MAY</t>
+          <t>MUST</t>
         </is>
       </c>
     </row>
@@ -5062,7 +5066,7 @@
       <c r="B146" s="2" t="n"/>
       <c r="C146" s="2" t="inlineStr">
         <is>
-          <t>Applicant signature</t>
+          <t>Ownership certificate type</t>
         </is>
       </c>
       <c r="D146" s="2" t="inlineStr"/>
@@ -5070,12 +5074,12 @@
       <c r="F146" s="2" t="inlineStr"/>
       <c r="G146" s="2" t="inlineStr">
         <is>
-          <t>Digital signature of the applicant</t>
+          <t>The type of ownership certificate based on ownership and tenancy status</t>
         </is>
       </c>
       <c r="H146" s="2" t="inlineStr">
         <is>
-          <t>string</t>
+          <t>enum</t>
         </is>
       </c>
       <c r="I146" s="2" t="inlineStr">
@@ -5089,7 +5093,7 @@
       <c r="B147" s="2" t="n"/>
       <c r="C147" s="2" t="inlineStr">
         <is>
-          <t>Agent signature</t>
+          <t>Applicant signature</t>
         </is>
       </c>
       <c r="D147" s="2" t="inlineStr"/>
@@ -5097,7 +5101,7 @@
       <c r="F147" s="2" t="inlineStr"/>
       <c r="G147" s="2" t="inlineStr">
         <is>
-          <t>Digital signature of the agent (if applicable)</t>
+          <t>Digital signature of the applicant</t>
         </is>
       </c>
       <c r="H147" s="2" t="inlineStr">
@@ -5116,7 +5120,7 @@
       <c r="B148" s="2" t="n"/>
       <c r="C148" s="2" t="inlineStr">
         <is>
-          <t>Signature date</t>
+          <t>Agent signature</t>
         </is>
       </c>
       <c r="D148" s="2" t="inlineStr"/>
@@ -5124,12 +5128,12 @@
       <c r="F148" s="2" t="inlineStr"/>
       <c r="G148" s="2" t="inlineStr">
         <is>
-          <t>Date when the ownership certificate was signed</t>
+          <t>Digital signature of the agent (if applicable)</t>
         </is>
       </c>
       <c r="H148" s="2" t="inlineStr">
         <is>
-          <t>date</t>
+          <t>string</t>
         </is>
       </c>
       <c r="I148" s="2" t="inlineStr">
@@ -5139,19 +5143,11 @@
       </c>
     </row>
     <row r="149">
-      <c r="A149" s="2" t="inlineStr">
-        <is>
-          <t>Pre-application advice</t>
-        </is>
-      </c>
-      <c r="B149" s="2" t="inlineStr">
-        <is>
-          <t>Details of pre-application advice previously received from the planning authority</t>
-        </is>
-      </c>
+      <c r="A149" s="2" t="n"/>
+      <c r="B149" s="2" t="n"/>
       <c r="C149" s="2" t="inlineStr">
         <is>
-          <t>Pre-application advice sought</t>
+          <t>Signature date</t>
         </is>
       </c>
       <c r="D149" s="2" t="inlineStr"/>
@@ -5159,26 +5155,34 @@
       <c r="F149" s="2" t="inlineStr"/>
       <c r="G149" s="2" t="inlineStr">
         <is>
-          <t>Whether pre-application advice has been sought from the planning authority</t>
+          <t>Date when the ownership certificate was signed</t>
         </is>
       </c>
       <c r="H149" s="2" t="inlineStr">
         <is>
-          <t>boolean</t>
+          <t>date</t>
         </is>
       </c>
       <c r="I149" s="2" t="inlineStr">
         <is>
-          <t>MUST</t>
+          <t>MAY</t>
         </is>
       </c>
     </row>
     <row r="150">
-      <c r="A150" s="2" t="n"/>
-      <c r="B150" s="2" t="n"/>
+      <c r="A150" s="2" t="inlineStr">
+        <is>
+          <t>Pre-application advice</t>
+        </is>
+      </c>
+      <c r="B150" s="2" t="inlineStr">
+        <is>
+          <t>Details of pre-application advice previously received from the planning authority</t>
+        </is>
+      </c>
       <c r="C150" s="2" t="inlineStr">
         <is>
-          <t>Officer name</t>
+          <t>Pre-application advice sought</t>
         </is>
       </c>
       <c r="D150" s="2" t="inlineStr"/>
@@ -5186,17 +5190,17 @@
       <c r="F150" s="2" t="inlineStr"/>
       <c r="G150" s="2" t="inlineStr">
         <is>
-          <t>Name of the planning officer who provided the pre-application advice</t>
+          <t>Whether pre-application advice has been sought from the planning authority</t>
         </is>
       </c>
       <c r="H150" s="2" t="inlineStr">
         <is>
-          <t>string</t>
+          <t>boolean</t>
         </is>
       </c>
       <c r="I150" s="2" t="inlineStr">
         <is>
-          <t>MAY</t>
+          <t>MUST</t>
         </is>
       </c>
     </row>
@@ -5205,7 +5209,7 @@
       <c r="B151" s="2" t="n"/>
       <c r="C151" s="2" t="inlineStr">
         <is>
-          <t>Reference</t>
+          <t>Officer name</t>
         </is>
       </c>
       <c r="D151" s="2" t="inlineStr"/>
@@ -5213,7 +5217,7 @@
       <c r="F151" s="2" t="inlineStr"/>
       <c r="G151" s="2" t="inlineStr">
         <is>
-          <t>A unique reference for the data item</t>
+          <t>Name of the planning officer who provided the pre-application advice</t>
         </is>
       </c>
       <c r="H151" s="2" t="inlineStr">
@@ -5232,7 +5236,7 @@
       <c r="B152" s="2" t="n"/>
       <c r="C152" s="2" t="inlineStr">
         <is>
-          <t>Advice date</t>
+          <t>Reference</t>
         </is>
       </c>
       <c r="D152" s="2" t="inlineStr"/>
@@ -5240,7 +5244,7 @@
       <c r="F152" s="2" t="inlineStr"/>
       <c r="G152" s="2" t="inlineStr">
         <is>
-          <t>Date when pre-application advice was received, in YYYY-MM-DD format</t>
+          <t>A unique reference for the data item</t>
         </is>
       </c>
       <c r="H152" s="2" t="inlineStr">
@@ -5259,7 +5263,7 @@
       <c r="B153" s="2" t="n"/>
       <c r="C153" s="2" t="inlineStr">
         <is>
-          <t>Advice summary</t>
+          <t>Advice date</t>
         </is>
       </c>
       <c r="D153" s="2" t="inlineStr"/>
@@ -5267,7 +5271,7 @@
       <c r="F153" s="2" t="inlineStr"/>
       <c r="G153" s="2" t="inlineStr">
         <is>
-          <t>Summary of the pre-application advice received from the planning authority</t>
+          <t>Date when pre-application advice was received, in YYYY-MM-DD format</t>
         </is>
       </c>
       <c r="H153" s="2" t="inlineStr">
@@ -5282,19 +5286,11 @@
       </c>
     </row>
     <row r="154">
-      <c r="A154" s="2" t="inlineStr">
-        <is>
-          <t>Processes machinery waste</t>
-        </is>
-      </c>
-      <c r="B154" s="2" t="inlineStr">
-        <is>
-          <t>How waste will be managed on the site</t>
-        </is>
-      </c>
+      <c r="A154" s="2" t="n"/>
+      <c r="B154" s="2" t="n"/>
       <c r="C154" s="2" t="inlineStr">
         <is>
-          <t>Site activity details</t>
+          <t>Advice summary</t>
         </is>
       </c>
       <c r="D154" s="2" t="inlineStr"/>
@@ -5302,7 +5298,7 @@
       <c r="F154" s="2" t="inlineStr"/>
       <c r="G154" s="2" t="inlineStr">
         <is>
-          <t>Description of activities, processes, and end products including site operations, plant, ventilation, and machinery</t>
+          <t>Summary of the pre-application advice received from the planning authority</t>
         </is>
       </c>
       <c r="H154" s="2" t="inlineStr">
@@ -5312,16 +5308,24 @@
       </c>
       <c r="I154" s="2" t="inlineStr">
         <is>
-          <t>MUST</t>
+          <t>MAY</t>
         </is>
       </c>
     </row>
     <row r="155">
-      <c r="A155" s="2" t="n"/>
-      <c r="B155" s="2" t="n"/>
+      <c r="A155" s="2" t="inlineStr">
+        <is>
+          <t>Processes machinery waste</t>
+        </is>
+      </c>
+      <c r="B155" s="2" t="inlineStr">
+        <is>
+          <t>How waste will be managed on the site</t>
+        </is>
+      </c>
       <c r="C155" s="2" t="inlineStr">
         <is>
-          <t>Proposal waste management</t>
+          <t>Site activity details</t>
         </is>
       </c>
       <c r="D155" s="2" t="inlineStr"/>
@@ -5329,12 +5333,12 @@
       <c r="F155" s="2" t="inlineStr"/>
       <c r="G155" s="2" t="inlineStr">
         <is>
-          <t>Whether the proposal involves waste management development</t>
+          <t>Description of activities, processes, and end products including site operations, plant, ventilation, and machinery</t>
         </is>
       </c>
       <c r="H155" s="2" t="inlineStr">
         <is>
-          <t>boolean</t>
+          <t>string</t>
         </is>
       </c>
       <c r="I155" s="2" t="inlineStr">
@@ -5348,24 +5352,20 @@
       <c r="B156" s="2" t="n"/>
       <c r="C156" s="2" t="inlineStr">
         <is>
-          <t>Waste management[]</t>
-        </is>
-      </c>
-      <c r="D156" s="2" t="inlineStr">
-        <is>
-          <t>Waste management facility type</t>
-        </is>
-      </c>
+          <t>Proposal waste management</t>
+        </is>
+      </c>
+      <c r="D156" s="2" t="inlineStr"/>
       <c r="E156" s="2" t="inlineStr"/>
       <c r="F156" s="2" t="inlineStr"/>
       <c r="G156" s="2" t="inlineStr">
         <is>
-          <t>Type of waste management facility</t>
+          <t>Whether the proposal involves waste management development</t>
         </is>
       </c>
       <c r="H156" s="2" t="inlineStr">
         <is>
-          <t>enum</t>
+          <t>boolean</t>
         </is>
       </c>
       <c r="I156" s="2" t="inlineStr">
@@ -5384,24 +5384,24 @@
       </c>
       <c r="D157" s="2" t="inlineStr">
         <is>
-          <t>Not applicable</t>
+          <t>Waste management facility type</t>
         </is>
       </c>
       <c r="E157" s="2" t="inlineStr"/>
       <c r="F157" s="2" t="inlineStr"/>
       <c r="G157" s="2" t="inlineStr">
         <is>
-          <t>Whether the facility is not applicable</t>
+          <t>Type of waste management facility</t>
         </is>
       </c>
       <c r="H157" s="2" t="inlineStr">
         <is>
-          <t>boolean</t>
+          <t>enum</t>
         </is>
       </c>
       <c r="I157" s="2" t="inlineStr">
         <is>
-          <t>MAY</t>
+          <t>MUST</t>
         </is>
       </c>
     </row>
@@ -5415,19 +5415,19 @@
       </c>
       <c r="D158" s="2" t="inlineStr">
         <is>
-          <t>Total capacity</t>
+          <t>Not applicable</t>
         </is>
       </c>
       <c r="E158" s="2" t="inlineStr"/>
       <c r="F158" s="2" t="inlineStr"/>
       <c r="G158" s="2" t="inlineStr">
         <is>
-          <t>Total capacity of void in cubic metres (or tonnes/litres)</t>
+          <t>Whether the facility is not applicable</t>
         </is>
       </c>
       <c r="H158" s="2" t="inlineStr">
         <is>
-          <t>number</t>
+          <t>boolean</t>
         </is>
       </c>
       <c r="I158" s="2" t="inlineStr">
@@ -5446,14 +5446,14 @@
       </c>
       <c r="D159" s="2" t="inlineStr">
         <is>
-          <t>Annual throughput</t>
+          <t>Total capacity</t>
         </is>
       </c>
       <c r="E159" s="2" t="inlineStr"/>
       <c r="F159" s="2" t="inlineStr"/>
       <c r="G159" s="2" t="inlineStr">
         <is>
-          <t>Maximum annual operational throughput in tonnes/litres</t>
+          <t>Total capacity of void in cubic metres (or tonnes/litres)</t>
         </is>
       </c>
       <c r="H159" s="2" t="inlineStr">
@@ -5472,19 +5472,19 @@
       <c r="B160" s="2" t="n"/>
       <c r="C160" s="2" t="inlineStr">
         <is>
-          <t>Waste streams throughput</t>
+          <t>Waste management[]</t>
         </is>
       </c>
       <c r="D160" s="2" t="inlineStr">
         <is>
-          <t>Municipal</t>
+          <t>Annual throughput</t>
         </is>
       </c>
       <c r="E160" s="2" t="inlineStr"/>
       <c r="F160" s="2" t="inlineStr"/>
       <c r="G160" s="2" t="inlineStr">
         <is>
-          <t>Maximum throughput for municipal waste (annual throughput in tonnes/litres)</t>
+          <t>Maximum annual operational throughput in tonnes/litres</t>
         </is>
       </c>
       <c r="H160" s="2" t="inlineStr">
@@ -5508,14 +5508,14 @@
       </c>
       <c r="D161" s="2" t="inlineStr">
         <is>
-          <t>Construction demolition</t>
+          <t>Municipal</t>
         </is>
       </c>
       <c r="E161" s="2" t="inlineStr"/>
       <c r="F161" s="2" t="inlineStr"/>
       <c r="G161" s="2" t="inlineStr">
         <is>
-          <t>Maximum throughput for construction and demolition waste (annual throughput in tonnes/litres)</t>
+          <t>Maximum throughput for municipal waste (annual throughput in tonnes/litres)</t>
         </is>
       </c>
       <c r="H161" s="2" t="inlineStr">
@@ -5539,14 +5539,14 @@
       </c>
       <c r="D162" s="2" t="inlineStr">
         <is>
-          <t>Commercial industrial</t>
+          <t>Construction demolition</t>
         </is>
       </c>
       <c r="E162" s="2" t="inlineStr"/>
       <c r="F162" s="2" t="inlineStr"/>
       <c r="G162" s="2" t="inlineStr">
         <is>
-          <t>Maximum throughput for commercial and industrial waste (annual throughput in tonnes/litres)</t>
+          <t>Maximum throughput for construction and demolition waste (annual throughput in tonnes/litres)</t>
         </is>
       </c>
       <c r="H162" s="2" t="inlineStr">
@@ -5570,14 +5570,14 @@
       </c>
       <c r="D163" s="2" t="inlineStr">
         <is>
-          <t>Hazardous</t>
+          <t>Commercial industrial</t>
         </is>
       </c>
       <c r="E163" s="2" t="inlineStr"/>
       <c r="F163" s="2" t="inlineStr"/>
       <c r="G163" s="2" t="inlineStr">
         <is>
-          <t>Maximum throughput for hazardous waste (annual throughput in tonnes/litres)</t>
+          <t>Maximum throughput for commercial and industrial waste (annual throughput in tonnes/litres)</t>
         </is>
       </c>
       <c r="H163" s="2" t="inlineStr">
@@ -5592,46 +5592,50 @@
       </c>
     </row>
     <row r="164">
-      <c r="A164" s="2" t="inlineStr">
-        <is>
-          <t>Description of the proposal</t>
-        </is>
-      </c>
-      <c r="B164" s="2" t="inlineStr">
-        <is>
-          <t>What development, works or change of use is proposed</t>
-        </is>
-      </c>
+      <c r="A164" s="2" t="n"/>
+      <c r="B164" s="2" t="n"/>
       <c r="C164" s="2" t="inlineStr">
         <is>
-          <t>Proposal description</t>
-        </is>
-      </c>
-      <c r="D164" s="2" t="inlineStr"/>
+          <t>Waste streams throughput</t>
+        </is>
+      </c>
+      <c r="D164" s="2" t="inlineStr">
+        <is>
+          <t>Hazardous</t>
+        </is>
+      </c>
       <c r="E164" s="2" t="inlineStr"/>
       <c r="F164" s="2" t="inlineStr"/>
       <c r="G164" s="2" t="inlineStr">
         <is>
-          <t>A description of what is being proposed, including the development, works, or change of use</t>
+          <t>Maximum throughput for hazardous waste (annual throughput in tonnes/litres)</t>
         </is>
       </c>
       <c r="H164" s="2" t="inlineStr">
         <is>
-          <t>string</t>
+          <t>number</t>
         </is>
       </c>
       <c r="I164" s="2" t="inlineStr">
         <is>
-          <t>MUST</t>
+          <t>MAY</t>
         </is>
       </c>
     </row>
     <row r="165">
-      <c r="A165" s="2" t="n"/>
-      <c r="B165" s="2" t="n"/>
+      <c r="A165" s="2" t="inlineStr">
+        <is>
+          <t>Description of the proposal</t>
+        </is>
+      </c>
+      <c r="B165" s="2" t="inlineStr">
+        <is>
+          <t>What development, works or change of use is proposed</t>
+        </is>
+      </c>
       <c r="C165" s="2" t="inlineStr">
         <is>
-          <t>Proposal started</t>
+          <t>Proposal description</t>
         </is>
       </c>
       <c r="D165" s="2" t="inlineStr"/>
@@ -5639,12 +5643,12 @@
       <c r="F165" s="2" t="inlineStr"/>
       <c r="G165" s="2" t="inlineStr">
         <is>
-          <t>Has any work on the proposal already been started</t>
+          <t>A description of what is being proposed, including the development, works, or change of use</t>
         </is>
       </c>
       <c r="H165" s="2" t="inlineStr">
         <is>
-          <t>boolean</t>
+          <t>string</t>
         </is>
       </c>
       <c r="I165" s="2" t="inlineStr">
@@ -5658,7 +5662,7 @@
       <c r="B166" s="2" t="n"/>
       <c r="C166" s="2" t="inlineStr">
         <is>
-          <t>Proposal start date</t>
+          <t>Proposal started</t>
         </is>
       </c>
       <c r="D166" s="2" t="inlineStr"/>
@@ -5666,17 +5670,17 @@
       <c r="F166" s="2" t="inlineStr"/>
       <c r="G166" s="2" t="inlineStr">
         <is>
-          <t>The date when work on the proposal started, in YYYY-MM-DD format</t>
+          <t>Has any work on the proposal already been started</t>
         </is>
       </c>
       <c r="H166" s="2" t="inlineStr">
         <is>
-          <t>date</t>
+          <t>boolean</t>
         </is>
       </c>
       <c r="I166" s="2" t="inlineStr">
         <is>
-          <t>MAY</t>
+          <t>MUST</t>
         </is>
       </c>
     </row>
@@ -5685,7 +5689,7 @@
       <c r="B167" s="2" t="n"/>
       <c r="C167" s="2" t="inlineStr">
         <is>
-          <t>Proposal completed</t>
+          <t>Proposal start date</t>
         </is>
       </c>
       <c r="D167" s="2" t="inlineStr"/>
@@ -5693,17 +5697,17 @@
       <c r="F167" s="2" t="inlineStr"/>
       <c r="G167" s="2" t="inlineStr">
         <is>
-          <t>Has any work on the proposal already been completed</t>
+          <t>The date when work on the proposal started, in YYYY-MM-DD format</t>
         </is>
       </c>
       <c r="H167" s="2" t="inlineStr">
         <is>
-          <t>boolean</t>
+          <t>date</t>
         </is>
       </c>
       <c r="I167" s="2" t="inlineStr">
         <is>
-          <t>MUST</t>
+          <t>MAY</t>
         </is>
       </c>
     </row>
@@ -5712,7 +5716,7 @@
       <c r="B168" s="2" t="n"/>
       <c r="C168" s="2" t="inlineStr">
         <is>
-          <t>Proposal completion date</t>
+          <t>Proposal completed</t>
         </is>
       </c>
       <c r="D168" s="2" t="inlineStr"/>
@@ -5720,17 +5724,17 @@
       <c r="F168" s="2" t="inlineStr"/>
       <c r="G168" s="2" t="inlineStr">
         <is>
-          <t>The date when work on the proposal was completed, in YYYY-MM-DD format</t>
+          <t>Has any work on the proposal already been completed</t>
         </is>
       </c>
       <c r="H168" s="2" t="inlineStr">
         <is>
-          <t>date</t>
+          <t>boolean</t>
         </is>
       </c>
       <c r="I168" s="2" t="inlineStr">
         <is>
-          <t>MAY</t>
+          <t>MUST</t>
         </is>
       </c>
     </row>
@@ -5739,7 +5743,7 @@
       <c r="B169" s="2" t="n"/>
       <c r="C169" s="2" t="inlineStr">
         <is>
-          <t>PIP reference</t>
+          <t>Proposal completion date</t>
         </is>
       </c>
       <c r="D169" s="2" t="inlineStr"/>
@@ -5747,12 +5751,12 @@
       <c r="F169" s="2" t="inlineStr"/>
       <c r="G169" s="2" t="inlineStr">
         <is>
-          <t>Reference number for the Planning in Principle (PIP) application this relates to</t>
+          <t>The date when work on the proposal was completed, in YYYY-MM-DD format</t>
         </is>
       </c>
       <c r="H169" s="2" t="inlineStr">
         <is>
-          <t>string</t>
+          <t>date</t>
         </is>
       </c>
       <c r="I169" s="2" t="inlineStr">
@@ -5766,7 +5770,7 @@
       <c r="B170" s="2" t="n"/>
       <c r="C170" s="2" t="inlineStr">
         <is>
-          <t>Is public service infrastructure</t>
+          <t>PIP reference</t>
         </is>
       </c>
       <c r="D170" s="2" t="inlineStr"/>
@@ -5774,34 +5778,26 @@
       <c r="F170" s="2" t="inlineStr"/>
       <c r="G170" s="2" t="inlineStr">
         <is>
-          <t>For applications made on or after 1 August 2021, is the proposal for public service infrastructure development</t>
+          <t>Reference number for the Planning in Principle (PIP) application this relates to</t>
         </is>
       </c>
       <c r="H170" s="2" t="inlineStr">
         <is>
-          <t>boolean</t>
+          <t>string</t>
         </is>
       </c>
       <c r="I170" s="2" t="inlineStr">
         <is>
-          <t>MUST</t>
+          <t>MAY</t>
         </is>
       </c>
     </row>
     <row r="171">
-      <c r="A171" s="2" t="inlineStr">
-        <is>
-          <t>Residential units</t>
-        </is>
-      </c>
-      <c r="B171" s="2" t="inlineStr">
-        <is>
-          <t>Details of the residential units that make up both the current and proposed development.</t>
-        </is>
-      </c>
+      <c r="A171" s="2" t="n"/>
+      <c r="B171" s="2" t="n"/>
       <c r="C171" s="2" t="inlineStr">
         <is>
-          <t>Residential unit change</t>
+          <t>Is public service infrastructure</t>
         </is>
       </c>
       <c r="D171" s="2" t="inlineStr"/>
@@ -5809,7 +5805,7 @@
       <c r="F171" s="2" t="inlineStr"/>
       <c r="G171" s="2" t="inlineStr">
         <is>
-          <t>Proposal includes the gain, loss or change of use of residential units</t>
+          <t>For applications made on or after 1 August 2021, is the proposal for public service infrastructure development</t>
         </is>
       </c>
       <c r="H171" s="2" t="inlineStr">
@@ -5824,28 +5820,32 @@
       </c>
     </row>
     <row r="172">
-      <c r="A172" s="2" t="n"/>
-      <c r="B172" s="2" t="n"/>
+      <c r="A172" s="2" t="inlineStr">
+        <is>
+          <t>Residential units</t>
+        </is>
+      </c>
+      <c r="B172" s="2" t="inlineStr">
+        <is>
+          <t>Details of the residential units that make up both the current and proposed development.</t>
+        </is>
+      </c>
       <c r="C172" s="2" t="inlineStr">
         <is>
-          <t>Residential unit summary[]</t>
-        </is>
-      </c>
-      <c r="D172" s="2" t="inlineStr">
-        <is>
-          <t>Tenure type</t>
-        </is>
-      </c>
+          <t>Residential unit change</t>
+        </is>
+      </c>
+      <c r="D172" s="2" t="inlineStr"/>
       <c r="E172" s="2" t="inlineStr"/>
       <c r="F172" s="2" t="inlineStr"/>
       <c r="G172" s="2" t="inlineStr">
         <is>
-          <t>Category of housing tenure</t>
+          <t>Proposal includes the gain, loss or change of use of residential units</t>
         </is>
       </c>
       <c r="H172" s="2" t="inlineStr">
         <is>
-          <t>enum</t>
+          <t>boolean</t>
         </is>
       </c>
       <c r="I172" s="2" t="inlineStr">
@@ -5864,14 +5864,14 @@
       </c>
       <c r="D173" s="2" t="inlineStr">
         <is>
-          <t>Housing type</t>
+          <t>Tenure type</t>
         </is>
       </c>
       <c r="E173" s="2" t="inlineStr"/>
       <c r="F173" s="2" t="inlineStr"/>
       <c r="G173" s="2" t="inlineStr">
         <is>
-          <t>Type of housing</t>
+          <t>Category of housing tenure</t>
         </is>
       </c>
       <c r="H173" s="2" t="inlineStr">
@@ -5895,23 +5895,19 @@
       </c>
       <c r="D174" s="2" t="inlineStr">
         <is>
-          <t>Existing unit breakdown[]</t>
-        </is>
-      </c>
-      <c r="E174" s="2" t="inlineStr">
-        <is>
-          <t>Units unknown</t>
-        </is>
-      </c>
+          <t>Housing type</t>
+        </is>
+      </c>
+      <c r="E174" s="2" t="inlineStr"/>
       <c r="F174" s="2" t="inlineStr"/>
       <c r="G174" s="2" t="inlineStr">
         <is>
-          <t>Whether the number of units is unknown</t>
+          <t>Type of housing</t>
         </is>
       </c>
       <c r="H174" s="2" t="inlineStr">
         <is>
-          <t>boolean</t>
+          <t>enum</t>
         </is>
       </c>
       <c r="I174" s="2" t="inlineStr">
@@ -5935,17 +5931,13 @@
       </c>
       <c r="E175" s="2" t="inlineStr">
         <is>
-          <t>Units per bedroom number[]</t>
-        </is>
-      </c>
-      <c r="F175" s="2" t="inlineStr">
-        <is>
-          <t>No bedrooms unknown</t>
-        </is>
-      </c>
+          <t>Units unknown</t>
+        </is>
+      </c>
+      <c r="F175" s="2" t="inlineStr"/>
       <c r="G175" s="2" t="inlineStr">
         <is>
-          <t>Set to true when counting units where bedroom number is unknown</t>
+          <t>Whether the number of units is unknown</t>
         </is>
       </c>
       <c r="H175" s="2" t="inlineStr">
@@ -5979,22 +5971,22 @@
       </c>
       <c r="F176" s="2" t="inlineStr">
         <is>
-          <t>Number of bedrooms</t>
+          <t>No bedrooms unknown</t>
         </is>
       </c>
       <c r="G176" s="2" t="inlineStr">
         <is>
-          <t>The number of bedrooms in unit</t>
+          <t>Set to true when counting units where bedroom number is unknown</t>
         </is>
       </c>
       <c r="H176" s="2" t="inlineStr">
         <is>
-          <t>number</t>
+          <t>boolean</t>
         </is>
       </c>
       <c r="I176" s="2" t="inlineStr">
         <is>
-          <t>MAY</t>
+          <t>MUST</t>
         </is>
       </c>
     </row>
@@ -6018,12 +6010,12 @@
       </c>
       <c r="F177" s="2" t="inlineStr">
         <is>
-          <t>Units</t>
+          <t>Number of bedrooms</t>
         </is>
       </c>
       <c r="G177" s="2" t="inlineStr">
         <is>
-          <t>The number of units of that bedroom count</t>
+          <t>The number of bedrooms in unit</t>
         </is>
       </c>
       <c r="H177" s="2" t="inlineStr">
@@ -6033,7 +6025,7 @@
       </c>
       <c r="I177" s="2" t="inlineStr">
         <is>
-          <t>MUST</t>
+          <t>MAY</t>
         </is>
       </c>
     </row>
@@ -6052,13 +6044,17 @@
       </c>
       <c r="E178" s="2" t="inlineStr">
         <is>
-          <t>Total units</t>
-        </is>
-      </c>
-      <c r="F178" s="2" t="inlineStr"/>
+          <t>Units per bedroom number[]</t>
+        </is>
+      </c>
+      <c r="F178" s="2" t="inlineStr">
+        <is>
+          <t>Units</t>
+        </is>
+      </c>
       <c r="G178" s="2" t="inlineStr">
         <is>
-          <t>Total number of units</t>
+          <t>The number of units of that bedroom count</t>
         </is>
       </c>
       <c r="H178" s="2" t="inlineStr">
@@ -6068,7 +6064,7 @@
       </c>
       <c r="I178" s="2" t="inlineStr">
         <is>
-          <t>MAY</t>
+          <t>MUST</t>
         </is>
       </c>
     </row>
@@ -6082,28 +6078,28 @@
       </c>
       <c r="D179" s="2" t="inlineStr">
         <is>
-          <t>Proposed unit breakdown[]</t>
+          <t>Existing unit breakdown[]</t>
         </is>
       </c>
       <c r="E179" s="2" t="inlineStr">
         <is>
-          <t>Units unknown</t>
+          <t>Total units</t>
         </is>
       </c>
       <c r="F179" s="2" t="inlineStr"/>
       <c r="G179" s="2" t="inlineStr">
         <is>
-          <t>Whether the number of units is unknown</t>
+          <t>Total number of units</t>
         </is>
       </c>
       <c r="H179" s="2" t="inlineStr">
         <is>
-          <t>boolean</t>
+          <t>number</t>
         </is>
       </c>
       <c r="I179" s="2" t="inlineStr">
         <is>
-          <t>MUST</t>
+          <t>MAY</t>
         </is>
       </c>
     </row>
@@ -6122,17 +6118,13 @@
       </c>
       <c r="E180" s="2" t="inlineStr">
         <is>
-          <t>Units per bedroom number[]</t>
-        </is>
-      </c>
-      <c r="F180" s="2" t="inlineStr">
-        <is>
-          <t>No bedrooms unknown</t>
-        </is>
-      </c>
+          <t>Units unknown</t>
+        </is>
+      </c>
+      <c r="F180" s="2" t="inlineStr"/>
       <c r="G180" s="2" t="inlineStr">
         <is>
-          <t>Set to true when counting units where bedroom number is unknown</t>
+          <t>Whether the number of units is unknown</t>
         </is>
       </c>
       <c r="H180" s="2" t="inlineStr">
@@ -6166,22 +6158,22 @@
       </c>
       <c r="F181" s="2" t="inlineStr">
         <is>
-          <t>Number of bedrooms</t>
+          <t>No bedrooms unknown</t>
         </is>
       </c>
       <c r="G181" s="2" t="inlineStr">
         <is>
-          <t>The number of bedrooms in unit</t>
+          <t>Set to true when counting units where bedroom number is unknown</t>
         </is>
       </c>
       <c r="H181" s="2" t="inlineStr">
         <is>
-          <t>number</t>
+          <t>boolean</t>
         </is>
       </c>
       <c r="I181" s="2" t="inlineStr">
         <is>
-          <t>MAY</t>
+          <t>MUST</t>
         </is>
       </c>
     </row>
@@ -6205,12 +6197,12 @@
       </c>
       <c r="F182" s="2" t="inlineStr">
         <is>
-          <t>Units</t>
+          <t>Number of bedrooms</t>
         </is>
       </c>
       <c r="G182" s="2" t="inlineStr">
         <is>
-          <t>The number of units of that bedroom count</t>
+          <t>The number of bedrooms in unit</t>
         </is>
       </c>
       <c r="H182" s="2" t="inlineStr">
@@ -6220,7 +6212,7 @@
       </c>
       <c r="I182" s="2" t="inlineStr">
         <is>
-          <t>MUST</t>
+          <t>MAY</t>
         </is>
       </c>
     </row>
@@ -6239,13 +6231,17 @@
       </c>
       <c r="E183" s="2" t="inlineStr">
         <is>
-          <t>Total units</t>
-        </is>
-      </c>
-      <c r="F183" s="2" t="inlineStr"/>
+          <t>Units per bedroom number[]</t>
+        </is>
+      </c>
+      <c r="F183" s="2" t="inlineStr">
+        <is>
+          <t>Units</t>
+        </is>
+      </c>
       <c r="G183" s="2" t="inlineStr">
         <is>
-          <t>Total number of units</t>
+          <t>The number of units of that bedroom count</t>
         </is>
       </c>
       <c r="H183" s="2" t="inlineStr">
@@ -6255,7 +6251,7 @@
       </c>
       <c r="I183" s="2" t="inlineStr">
         <is>
-          <t>MAY</t>
+          <t>MUST</t>
         </is>
       </c>
     </row>
@@ -6264,15 +6260,23 @@
       <c r="B184" s="2" t="n"/>
       <c r="C184" s="2" t="inlineStr">
         <is>
-          <t>Total existing units</t>
-        </is>
-      </c>
-      <c r="D184" s="2" t="inlineStr"/>
-      <c r="E184" s="2" t="inlineStr"/>
+          <t>Residential unit summary[]</t>
+        </is>
+      </c>
+      <c r="D184" s="2" t="inlineStr">
+        <is>
+          <t>Proposed unit breakdown[]</t>
+        </is>
+      </c>
+      <c r="E184" s="2" t="inlineStr">
+        <is>
+          <t>Total units</t>
+        </is>
+      </c>
       <c r="F184" s="2" t="inlineStr"/>
       <c r="G184" s="2" t="inlineStr">
         <is>
-          <t>The total number of existing units</t>
+          <t>Total number of units</t>
         </is>
       </c>
       <c r="H184" s="2" t="inlineStr">
@@ -6282,7 +6286,7 @@
       </c>
       <c r="I184" s="2" t="inlineStr">
         <is>
-          <t>MUST</t>
+          <t>MAY</t>
         </is>
       </c>
     </row>
@@ -6291,7 +6295,7 @@
       <c r="B185" s="2" t="n"/>
       <c r="C185" s="2" t="inlineStr">
         <is>
-          <t>Total proposed units</t>
+          <t>Total existing units</t>
         </is>
       </c>
       <c r="D185" s="2" t="inlineStr"/>
@@ -6299,7 +6303,7 @@
       <c r="F185" s="2" t="inlineStr"/>
       <c r="G185" s="2" t="inlineStr">
         <is>
-          <t>The total number of proposed units</t>
+          <t>The total number of existing units</t>
         </is>
       </c>
       <c r="H185" s="2" t="inlineStr">
@@ -6318,7 +6322,7 @@
       <c r="B186" s="2" t="n"/>
       <c r="C186" s="2" t="inlineStr">
         <is>
-          <t>Net change</t>
+          <t>Total proposed units</t>
         </is>
       </c>
       <c r="D186" s="2" t="inlineStr"/>
@@ -6326,7 +6330,7 @@
       <c r="F186" s="2" t="inlineStr"/>
       <c r="G186" s="2" t="inlineStr">
         <is>
-          <t>Calculated net change in units</t>
+          <t>The total number of proposed units</t>
         </is>
       </c>
       <c r="H186" s="2" t="inlineStr">
@@ -6341,19 +6345,11 @@
       </c>
     </row>
     <row r="187">
-      <c r="A187" s="2" t="inlineStr">
-        <is>
-          <t>Site area</t>
-        </is>
-      </c>
-      <c r="B187" s="2" t="inlineStr">
-        <is>
-          <t>How big the site is including relevant measurements</t>
-        </is>
-      </c>
+      <c r="A187" s="2" t="n"/>
+      <c r="B187" s="2" t="n"/>
       <c r="C187" s="2" t="inlineStr">
         <is>
-          <t>Site area in hectares</t>
+          <t>Net change</t>
         </is>
       </c>
       <c r="D187" s="2" t="inlineStr"/>
@@ -6361,7 +6357,7 @@
       <c r="F187" s="2" t="inlineStr"/>
       <c r="G187" s="2" t="inlineStr">
         <is>
-          <t>The size of the site in hectares</t>
+          <t>Calculated net change in units</t>
         </is>
       </c>
       <c r="H187" s="2" t="inlineStr">
@@ -6376,11 +6372,19 @@
       </c>
     </row>
     <row r="188">
-      <c r="A188" s="2" t="n"/>
-      <c r="B188" s="2" t="n"/>
+      <c r="A188" s="2" t="inlineStr">
+        <is>
+          <t>Site area</t>
+        </is>
+      </c>
+      <c r="B188" s="2" t="inlineStr">
+        <is>
+          <t>How big the site is including relevant measurements</t>
+        </is>
+      </c>
       <c r="C188" s="2" t="inlineStr">
         <is>
-          <t>Site area provided by</t>
+          <t>Site area in hectares</t>
         </is>
       </c>
       <c r="D188" s="2" t="inlineStr"/>
@@ -6388,51 +6392,39 @@
       <c r="F188" s="2" t="inlineStr"/>
       <c r="G188" s="2" t="inlineStr">
         <is>
-          <t>Who provided the site area value</t>
+          <t>The size of the site in hectares</t>
         </is>
       </c>
       <c r="H188" s="2" t="inlineStr">
         <is>
-          <t>enum</t>
+          <t>number</t>
         </is>
       </c>
       <c r="I188" s="2" t="inlineStr">
         <is>
-          <t>MAY</t>
+          <t>MUST</t>
         </is>
       </c>
     </row>
     <row r="189">
-      <c r="A189" s="2" t="inlineStr">
-        <is>
-          <t>Site details</t>
-        </is>
-      </c>
-      <c r="B189" s="2" t="inlineStr">
-        <is>
-          <t>Where the proposed development will be built.</t>
-        </is>
-      </c>
+      <c r="A189" s="2" t="n"/>
+      <c r="B189" s="2" t="n"/>
       <c r="C189" s="2" t="inlineStr">
         <is>
-          <t>Site locations[]</t>
-        </is>
-      </c>
-      <c r="D189" s="2" t="inlineStr">
-        <is>
-          <t>Site boundary</t>
-        </is>
-      </c>
+          <t>Site area provided by</t>
+        </is>
+      </c>
+      <c r="D189" s="2" t="inlineStr"/>
       <c r="E189" s="2" t="inlineStr"/>
       <c r="F189" s="2" t="inlineStr"/>
       <c r="G189" s="2" t="inlineStr">
         <is>
-          <t>Geometry of the site of the development, typically in GeoJSON format</t>
+          <t>Who provided the site area value</t>
         </is>
       </c>
       <c r="H189" s="2" t="inlineStr">
         <is>
-          <t>wkt</t>
+          <t>enum</t>
         </is>
       </c>
       <c r="I189" s="2" t="inlineStr">
@@ -6442,8 +6434,16 @@
       </c>
     </row>
     <row r="190">
-      <c r="A190" s="2" t="n"/>
-      <c r="B190" s="2" t="n"/>
+      <c r="A190" s="2" t="inlineStr">
+        <is>
+          <t>Site details</t>
+        </is>
+      </c>
+      <c r="B190" s="2" t="inlineStr">
+        <is>
+          <t>Where the proposed development will be built.</t>
+        </is>
+      </c>
       <c r="C190" s="2" t="inlineStr">
         <is>
           <t>Site locations[]</t>
@@ -6451,19 +6451,19 @@
       </c>
       <c r="D190" s="2" t="inlineStr">
         <is>
-          <t>Address Text</t>
+          <t>Site boundary</t>
         </is>
       </c>
       <c r="E190" s="2" t="inlineStr"/>
       <c r="F190" s="2" t="inlineStr"/>
       <c r="G190" s="2" t="inlineStr">
         <is>
-          <t>Flexible field for capturing addresses</t>
+          <t>Geometry of the site of the development, typically in GeoJSON format</t>
         </is>
       </c>
       <c r="H190" s="2" t="inlineStr">
         <is>
-          <t>string</t>
+          <t>wkt</t>
         </is>
       </c>
       <c r="I190" s="2" t="inlineStr">
@@ -6482,14 +6482,14 @@
       </c>
       <c r="D191" s="2" t="inlineStr">
         <is>
-          <t>Postcode</t>
+          <t>Address Text</t>
         </is>
       </c>
       <c r="E191" s="2" t="inlineStr"/>
       <c r="F191" s="2" t="inlineStr"/>
       <c r="G191" s="2" t="inlineStr">
         <is>
-          <t>The postal code</t>
+          <t>Flexible field for capturing addresses</t>
         </is>
       </c>
       <c r="H191" s="2" t="inlineStr">
@@ -6513,19 +6513,19 @@
       </c>
       <c r="D192" s="2" t="inlineStr">
         <is>
-          <t>Easting</t>
+          <t>Postcode</t>
         </is>
       </c>
       <c r="E192" s="2" t="inlineStr"/>
       <c r="F192" s="2" t="inlineStr"/>
       <c r="G192" s="2" t="inlineStr">
         <is>
-          <t>Easting coordinate in British National Grid (EPSG:27700)</t>
+          <t>The postal code</t>
         </is>
       </c>
       <c r="H192" s="2" t="inlineStr">
         <is>
-          <t>number</t>
+          <t>string</t>
         </is>
       </c>
       <c r="I192" s="2" t="inlineStr">
@@ -6544,14 +6544,14 @@
       </c>
       <c r="D193" s="2" t="inlineStr">
         <is>
-          <t>Northing</t>
+          <t>Easting</t>
         </is>
       </c>
       <c r="E193" s="2" t="inlineStr"/>
       <c r="F193" s="2" t="inlineStr"/>
       <c r="G193" s="2" t="inlineStr">
         <is>
-          <t>Northing coordinate in British National Grid (EPSG:27700)</t>
+          <t>Easting coordinate in British National Grid (EPSG:27700)</t>
         </is>
       </c>
       <c r="H193" s="2" t="inlineStr">
@@ -6575,14 +6575,14 @@
       </c>
       <c r="D194" s="2" t="inlineStr">
         <is>
-          <t>Latitude</t>
+          <t>Northing</t>
         </is>
       </c>
       <c r="E194" s="2" t="inlineStr"/>
       <c r="F194" s="2" t="inlineStr"/>
       <c r="G194" s="2" t="inlineStr">
         <is>
-          <t>Latitude coordinate in WGS84 (EPSG:4326)</t>
+          <t>Northing coordinate in British National Grid (EPSG:27700)</t>
         </is>
       </c>
       <c r="H194" s="2" t="inlineStr">
@@ -6606,14 +6606,14 @@
       </c>
       <c r="D195" s="2" t="inlineStr">
         <is>
-          <t>Longitude</t>
+          <t>Latitude</t>
         </is>
       </c>
       <c r="E195" s="2" t="inlineStr"/>
       <c r="F195" s="2" t="inlineStr"/>
       <c r="G195" s="2" t="inlineStr">
         <is>
-          <t>Longitude coordinate in WGS84 (EPSG:4326)</t>
+          <t>Latitude coordinate in WGS84 (EPSG:4326)</t>
         </is>
       </c>
       <c r="H195" s="2" t="inlineStr">
@@ -6637,19 +6637,19 @@
       </c>
       <c r="D196" s="2" t="inlineStr">
         <is>
-          <t>Description</t>
+          <t>Longitude</t>
         </is>
       </c>
       <c r="E196" s="2" t="inlineStr"/>
       <c r="F196" s="2" t="inlineStr"/>
       <c r="G196" s="2" t="inlineStr">
         <is>
-          <t>A text description providing details about the subject. For parking changes, this describes how the proposed works affect existing car parking arrangements.</t>
+          <t>Longitude coordinate in WGS84 (EPSG:4326)</t>
         </is>
       </c>
       <c r="H196" s="2" t="inlineStr">
         <is>
-          <t>string</t>
+          <t>number</t>
         </is>
       </c>
       <c r="I196" s="2" t="inlineStr">
@@ -6668,14 +6668,14 @@
       </c>
       <c r="D197" s="2" t="inlineStr">
         <is>
-          <t>UPRNs[]</t>
+          <t>Description</t>
         </is>
       </c>
       <c r="E197" s="2" t="inlineStr"/>
       <c r="F197" s="2" t="inlineStr"/>
       <c r="G197" s="2" t="inlineStr">
         <is>
-          <t>Unique Property Reference Numbers (UPRNs) for properties within the site boundary</t>
+          <t>A text description providing details about the subject. For parking changes, this describes how the proposed works affect existing car parking arrangements.</t>
         </is>
       </c>
       <c r="H197" s="2" t="inlineStr">
@@ -6690,46 +6690,50 @@
       </c>
     </row>
     <row r="198">
-      <c r="A198" s="2" t="inlineStr">
-        <is>
-          <t>Site Visit Details</t>
-        </is>
-      </c>
-      <c r="B198" s="2" t="inlineStr">
-        <is>
-          <t>Information to help the planning authority arrange a site visit</t>
-        </is>
-      </c>
+      <c r="A198" s="2" t="n"/>
+      <c r="B198" s="2" t="n"/>
       <c r="C198" s="2" t="inlineStr">
         <is>
-          <t>Site seen from public area</t>
-        </is>
-      </c>
-      <c r="D198" s="2" t="inlineStr"/>
+          <t>Site locations[]</t>
+        </is>
+      </c>
+      <c r="D198" s="2" t="inlineStr">
+        <is>
+          <t>UPRNs[]</t>
+        </is>
+      </c>
       <c r="E198" s="2" t="inlineStr"/>
       <c r="F198" s="2" t="inlineStr"/>
       <c r="G198" s="2" t="inlineStr">
         <is>
-          <t>Can site be seen from a public road, public footpath, bridleway or other public land</t>
+          <t>Unique Property Reference Numbers (UPRNs) for properties within the site boundary</t>
         </is>
       </c>
       <c r="H198" s="2" t="inlineStr">
         <is>
-          <t>boolean</t>
+          <t>string</t>
         </is>
       </c>
       <c r="I198" s="2" t="inlineStr">
         <is>
-          <t>MUST</t>
+          <t>MAY</t>
         </is>
       </c>
     </row>
     <row r="199">
-      <c r="A199" s="2" t="n"/>
-      <c r="B199" s="2" t="n"/>
+      <c r="A199" s="2" t="inlineStr">
+        <is>
+          <t>Site Visit Details</t>
+        </is>
+      </c>
+      <c r="B199" s="2" t="inlineStr">
+        <is>
+          <t>Information to help the planning authority arrange a site visit</t>
+        </is>
+      </c>
       <c r="C199" s="2" t="inlineStr">
         <is>
-          <t>Site visit contact type</t>
+          <t>Site seen from public area</t>
         </is>
       </c>
       <c r="D199" s="2" t="inlineStr"/>
@@ -6737,12 +6741,12 @@
       <c r="F199" s="2" t="inlineStr"/>
       <c r="G199" s="2" t="inlineStr">
         <is>
-          <t>Indicates who the authority should contact to arrange a site visit</t>
+          <t>Can site be seen from a public road, public footpath, bridleway or other public land</t>
         </is>
       </c>
       <c r="H199" s="2" t="inlineStr">
         <is>
-          <t>enum</t>
+          <t>boolean</t>
         </is>
       </c>
       <c r="I199" s="2" t="inlineStr">
@@ -6756,7 +6760,7 @@
       <c r="B200" s="2" t="n"/>
       <c r="C200" s="2" t="inlineStr">
         <is>
-          <t>Contact reference</t>
+          <t>Site visit contact type</t>
         </is>
       </c>
       <c r="D200" s="2" t="inlineStr"/>
@@ -6764,17 +6768,17 @@
       <c r="F200" s="2" t="inlineStr"/>
       <c r="G200" s="2" t="inlineStr">
         <is>
-          <t>The reference of the applicant or agent who should be contacted for site visits</t>
+          <t>Indicates who the authority should contact to arrange a site visit</t>
         </is>
       </c>
       <c r="H200" s="2" t="inlineStr">
         <is>
-          <t>string</t>
+          <t>enum</t>
         </is>
       </c>
       <c r="I200" s="2" t="inlineStr">
         <is>
-          <t>MAY</t>
+          <t>MUST</t>
         </is>
       </c>
     </row>
@@ -6783,19 +6787,15 @@
       <c r="B201" s="2" t="n"/>
       <c r="C201" s="2" t="inlineStr">
         <is>
-          <t>Other site visit contact</t>
-        </is>
-      </c>
-      <c r="D201" s="2" t="inlineStr">
-        <is>
-          <t>Full name</t>
-        </is>
-      </c>
+          <t>Contact reference</t>
+        </is>
+      </c>
+      <c r="D201" s="2" t="inlineStr"/>
       <c r="E201" s="2" t="inlineStr"/>
       <c r="F201" s="2" t="inlineStr"/>
       <c r="G201" s="2" t="inlineStr">
         <is>
-          <t>The complete name of a person</t>
+          <t>The reference of the applicant or agent who should be contacted for site visits</t>
         </is>
       </c>
       <c r="H201" s="2" t="inlineStr">
@@ -6805,7 +6805,7 @@
       </c>
       <c r="I201" s="2" t="inlineStr">
         <is>
-          <t>MUST</t>
+          <t>MAY</t>
         </is>
       </c>
     </row>
@@ -6819,14 +6819,14 @@
       </c>
       <c r="D202" s="2" t="inlineStr">
         <is>
-          <t>Phone number</t>
+          <t>Full name</t>
         </is>
       </c>
       <c r="E202" s="2" t="inlineStr"/>
       <c r="F202" s="2" t="inlineStr"/>
       <c r="G202" s="2" t="inlineStr">
         <is>
-          <t>A phone number</t>
+          <t>The complete name of a person</t>
         </is>
       </c>
       <c r="H202" s="2" t="inlineStr">
@@ -6850,14 +6850,14 @@
       </c>
       <c r="D203" s="2" t="inlineStr">
         <is>
-          <t>Email</t>
+          <t>Phone number</t>
         </is>
       </c>
       <c r="E203" s="2" t="inlineStr"/>
       <c r="F203" s="2" t="inlineStr"/>
       <c r="G203" s="2" t="inlineStr">
         <is>
-          <t>The email address that can be used for electronic correspondence with the individual</t>
+          <t>A phone number</t>
         </is>
       </c>
       <c r="H203" s="2" t="inlineStr">
@@ -6872,32 +6872,28 @@
       </c>
     </row>
     <row r="204">
-      <c r="A204" s="2" t="inlineStr">
-        <is>
-          <t>Trade effluent</t>
-        </is>
-      </c>
-      <c r="B204" s="2" t="inlineStr">
-        <is>
-          <t>Details of any liquid waste produced by industial processes on the proposed site, and how it will be diposed of.</t>
-        </is>
-      </c>
+      <c r="A204" s="2" t="n"/>
+      <c r="B204" s="2" t="n"/>
       <c r="C204" s="2" t="inlineStr">
         <is>
-          <t>Disposal required</t>
-        </is>
-      </c>
-      <c r="D204" s="2" t="inlineStr"/>
+          <t>Other site visit contact</t>
+        </is>
+      </c>
+      <c r="D204" s="2" t="inlineStr">
+        <is>
+          <t>Email</t>
+        </is>
+      </c>
       <c r="E204" s="2" t="inlineStr"/>
       <c r="F204" s="2" t="inlineStr"/>
       <c r="G204" s="2" t="inlineStr">
         <is>
-          <t>Does the proposal involve the disposal of trade effluents or waste (true/false)</t>
+          <t>The email address that can be used for electronic correspondence with the individual</t>
         </is>
       </c>
       <c r="H204" s="2" t="inlineStr">
         <is>
-          <t>boolean</t>
+          <t>string</t>
         </is>
       </c>
       <c r="I204" s="2" t="inlineStr">
@@ -6907,11 +6903,19 @@
       </c>
     </row>
     <row r="205">
-      <c r="A205" s="2" t="n"/>
-      <c r="B205" s="2" t="n"/>
+      <c r="A205" s="2" t="inlineStr">
+        <is>
+          <t>Trade effluent</t>
+        </is>
+      </c>
+      <c r="B205" s="2" t="inlineStr">
+        <is>
+          <t>Details of any liquid waste produced by industial processes on the proposed site, and how it will be diposed of.</t>
+        </is>
+      </c>
       <c r="C205" s="2" t="inlineStr">
         <is>
-          <t>Description</t>
+          <t>Disposal required</t>
         </is>
       </c>
       <c r="D205" s="2" t="inlineStr"/>
@@ -6919,34 +6923,26 @@
       <c r="F205" s="2" t="inlineStr"/>
       <c r="G205" s="2" t="inlineStr">
         <is>
-          <t>describe the nature, volume and means of disposal of trade effluents or waste</t>
+          <t>Does the proposal involve the disposal of trade effluents or waste (true/false)</t>
         </is>
       </c>
       <c r="H205" s="2" t="inlineStr">
         <is>
-          <t>string</t>
+          <t>boolean</t>
         </is>
       </c>
       <c r="I205" s="2" t="inlineStr">
         <is>
-          <t>MAY</t>
+          <t>MUST</t>
         </is>
       </c>
     </row>
     <row r="206">
-      <c r="A206" s="2" t="inlineStr">
-        <is>
-          <t>Trees and hedges information</t>
-        </is>
-      </c>
-      <c r="B206" s="2" t="inlineStr">
-        <is>
-          <t>Details of trees and/or hedges that will be affected by the proposed development</t>
-        </is>
-      </c>
+      <c r="A206" s="2" t="n"/>
+      <c r="B206" s="2" t="n"/>
       <c r="C206" s="2" t="inlineStr">
         <is>
-          <t>Trees on site</t>
+          <t>Description</t>
         </is>
       </c>
       <c r="D206" s="2" t="inlineStr"/>
@@ -6954,26 +6950,34 @@
       <c r="F206" s="2" t="inlineStr"/>
       <c r="G206" s="2" t="inlineStr">
         <is>
-          <t>Whether trees or hedges are present on the proposed development site</t>
+          <t>describe the nature, volume and means of disposal of trade effluents or waste</t>
         </is>
       </c>
       <c r="H206" s="2" t="inlineStr">
         <is>
-          <t>boolean</t>
+          <t>string</t>
         </is>
       </c>
       <c r="I206" s="2" t="inlineStr">
         <is>
-          <t>MUST</t>
+          <t>MAY</t>
         </is>
       </c>
     </row>
     <row r="207">
-      <c r="A207" s="2" t="n"/>
-      <c r="B207" s="2" t="n"/>
+      <c r="A207" s="2" t="inlineStr">
+        <is>
+          <t>Trees and hedges information</t>
+        </is>
+      </c>
+      <c r="B207" s="2" t="inlineStr">
+        <is>
+          <t>Details of trees and/or hedges that will be affected by the proposed development</t>
+        </is>
+      </c>
       <c r="C207" s="2" t="inlineStr">
         <is>
-          <t>Trees on adjacent land</t>
+          <t>Trees on site</t>
         </is>
       </c>
       <c r="D207" s="2" t="inlineStr"/>
@@ -6981,7 +6985,7 @@
       <c r="F207" s="2" t="inlineStr"/>
       <c r="G207" s="2" t="inlineStr">
         <is>
-          <t>Whether trees or hedges on land adjacent to the proposed development site could influence the development or might be important as part of the local landscape character</t>
+          <t>Whether trees or hedges are present on the proposed development site</t>
         </is>
       </c>
       <c r="H207" s="2" t="inlineStr">
@@ -6996,36 +7000,24 @@
       </c>
     </row>
     <row r="208">
-      <c r="A208" s="2" t="inlineStr">
-        <is>
-          <t>Vehicle parking</t>
-        </is>
-      </c>
-      <c r="B208" s="2" t="inlineStr">
-        <is>
-          <t>Details of current parking facilities at the site and any changes that would be made by the proposed development.</t>
-        </is>
-      </c>
+      <c r="A208" s="2" t="n"/>
+      <c r="B208" s="2" t="n"/>
       <c r="C208" s="2" t="inlineStr">
         <is>
-          <t>Parking spaces[]</t>
-        </is>
-      </c>
-      <c r="D208" s="2" t="inlineStr">
-        <is>
-          <t>Parking space type</t>
-        </is>
-      </c>
+          <t>Trees on adjacent land</t>
+        </is>
+      </c>
+      <c r="D208" s="2" t="inlineStr"/>
       <c r="E208" s="2" t="inlineStr"/>
       <c r="F208" s="2" t="inlineStr"/>
       <c r="G208" s="2" t="inlineStr">
         <is>
-          <t>Type of parking space or vehicle type</t>
+          <t>Whether trees or hedges on land adjacent to the proposed development site could influence the development or might be important as part of the local landscape character</t>
         </is>
       </c>
       <c r="H208" s="2" t="inlineStr">
         <is>
-          <t>enum</t>
+          <t>boolean</t>
         </is>
       </c>
       <c r="I208" s="2" t="inlineStr">
@@ -7035,8 +7027,16 @@
       </c>
     </row>
     <row r="209">
-      <c r="A209" s="2" t="n"/>
-      <c r="B209" s="2" t="n"/>
+      <c r="A209" s="2" t="inlineStr">
+        <is>
+          <t>Vehicle parking</t>
+        </is>
+      </c>
+      <c r="B209" s="2" t="inlineStr">
+        <is>
+          <t>Details of current parking facilities at the site and any changes that would be made by the proposed development.</t>
+        </is>
+      </c>
       <c r="C209" s="2" t="inlineStr">
         <is>
           <t>Parking spaces[]</t>
@@ -7044,24 +7044,24 @@
       </c>
       <c r="D209" s="2" t="inlineStr">
         <is>
-          <t>Vehicle type other</t>
+          <t>Parking space type</t>
         </is>
       </c>
       <c r="E209" s="2" t="inlineStr"/>
       <c r="F209" s="2" t="inlineStr"/>
       <c r="G209" s="2" t="inlineStr">
         <is>
-          <t>Vehicle type when parking space type is 'other'</t>
+          <t>Type of parking space or vehicle type</t>
         </is>
       </c>
       <c r="H209" s="2" t="inlineStr">
         <is>
-          <t>string</t>
+          <t>enum</t>
         </is>
       </c>
       <c r="I209" s="2" t="inlineStr">
         <is>
-          <t>MAY</t>
+          <t>MUST</t>
         </is>
       </c>
     </row>
@@ -7075,24 +7075,24 @@
       </c>
       <c r="D210" s="2" t="inlineStr">
         <is>
-          <t>Total existing</t>
+          <t>Vehicle type other</t>
         </is>
       </c>
       <c r="E210" s="2" t="inlineStr"/>
       <c r="F210" s="2" t="inlineStr"/>
       <c r="G210" s="2" t="inlineStr">
         <is>
-          <t>Total number of existing parking spaces</t>
+          <t>Vehicle type when parking space type is 'other'</t>
         </is>
       </c>
       <c r="H210" s="2" t="inlineStr">
         <is>
-          <t>number</t>
+          <t>string</t>
         </is>
       </c>
       <c r="I210" s="2" t="inlineStr">
         <is>
-          <t>MUST</t>
+          <t>MAY</t>
         </is>
       </c>
     </row>
@@ -7106,14 +7106,14 @@
       </c>
       <c r="D211" s="2" t="inlineStr">
         <is>
-          <t>Total proposed</t>
+          <t>Total existing</t>
         </is>
       </c>
       <c r="E211" s="2" t="inlineStr"/>
       <c r="F211" s="2" t="inlineStr"/>
       <c r="G211" s="2" t="inlineStr">
         <is>
-          <t>Total number of proposed parking spaces</t>
+          <t>Total number of existing parking spaces</t>
         </is>
       </c>
       <c r="H211" s="2" t="inlineStr">
@@ -7137,14 +7137,14 @@
       </c>
       <c r="D212" s="2" t="inlineStr">
         <is>
-          <t>Difference in spaces</t>
+          <t>Total proposed</t>
         </is>
       </c>
       <c r="E212" s="2" t="inlineStr"/>
       <c r="F212" s="2" t="inlineStr"/>
       <c r="G212" s="2" t="inlineStr">
         <is>
-          <t>Net change in parking spaces (proposed minus existing)</t>
+          <t>Total number of proposed parking spaces</t>
         </is>
       </c>
       <c r="H212" s="2" t="inlineStr">
@@ -7159,32 +7159,28 @@
       </c>
     </row>
     <row r="213">
-      <c r="A213" s="2" t="inlineStr">
-        <is>
-          <t>Waste storage and collection</t>
-        </is>
-      </c>
-      <c r="B213" s="2" t="inlineStr">
-        <is>
-          <t>Any waste storage or recycling arrangements are in place, such as waste storage areas</t>
-        </is>
-      </c>
+      <c r="A213" s="2" t="n"/>
+      <c r="B213" s="2" t="n"/>
       <c r="C213" s="2" t="inlineStr">
         <is>
-          <t>Needs waste storage area</t>
-        </is>
-      </c>
-      <c r="D213" s="2" t="inlineStr"/>
+          <t>Parking spaces[]</t>
+        </is>
+      </c>
+      <c r="D213" s="2" t="inlineStr">
+        <is>
+          <t>Difference in spaces</t>
+        </is>
+      </c>
       <c r="E213" s="2" t="inlineStr"/>
       <c r="F213" s="2" t="inlineStr"/>
       <c r="G213" s="2" t="inlineStr">
         <is>
-          <t>Does the proposal require a waste storage area</t>
+          <t>Net change in parking spaces (proposed minus existing)</t>
         </is>
       </c>
       <c r="H213" s="2" t="inlineStr">
         <is>
-          <t>boolean</t>
+          <t>number</t>
         </is>
       </c>
       <c r="I213" s="2" t="inlineStr">
@@ -7194,11 +7190,19 @@
       </c>
     </row>
     <row r="214">
-      <c r="A214" s="2" t="n"/>
-      <c r="B214" s="2" t="n"/>
+      <c r="A214" s="2" t="inlineStr">
+        <is>
+          <t>Waste storage and collection</t>
+        </is>
+      </c>
+      <c r="B214" s="2" t="inlineStr">
+        <is>
+          <t>Any waste storage or recycling arrangements are in place, such as waste storage areas</t>
+        </is>
+      </c>
       <c r="C214" s="2" t="inlineStr">
         <is>
-          <t>Waste storage area details</t>
+          <t>Needs waste storage area</t>
         </is>
       </c>
       <c r="D214" s="2" t="inlineStr"/>
@@ -7206,17 +7210,17 @@
       <c r="F214" s="2" t="inlineStr"/>
       <c r="G214" s="2" t="inlineStr">
         <is>
-          <t>Details of the waste storage area including location, size, design and access arrangements</t>
+          <t>Does the proposal require a waste storage area</t>
         </is>
       </c>
       <c r="H214" s="2" t="inlineStr">
         <is>
-          <t>string</t>
+          <t>boolean</t>
         </is>
       </c>
       <c r="I214" s="2" t="inlineStr">
         <is>
-          <t>MAY</t>
+          <t>MUST</t>
         </is>
       </c>
     </row>
@@ -7225,7 +7229,7 @@
       <c r="B215" s="2" t="n"/>
       <c r="C215" s="2" t="inlineStr">
         <is>
-          <t>Separate recycling arrangements</t>
+          <t>Waste storage area details</t>
         </is>
       </c>
       <c r="D215" s="2" t="inlineStr"/>
@@ -7233,17 +7237,17 @@
       <c r="F215" s="2" t="inlineStr"/>
       <c r="G215" s="2" t="inlineStr">
         <is>
-          <t>Does the proposal include separate recycling arrangements</t>
+          <t>Details of the waste storage area including location, size, design and access arrangements</t>
         </is>
       </c>
       <c r="H215" s="2" t="inlineStr">
         <is>
-          <t>boolean</t>
+          <t>string</t>
         </is>
       </c>
       <c r="I215" s="2" t="inlineStr">
         <is>
-          <t>MUST</t>
+          <t>MAY</t>
         </is>
       </c>
     </row>
@@ -7252,7 +7256,7 @@
       <c r="B216" s="2" t="n"/>
       <c r="C216" s="2" t="inlineStr">
         <is>
-          <t>Separate recycling arrangements details</t>
+          <t>Separate recycling arrangements</t>
         </is>
       </c>
       <c r="D216" s="2" t="inlineStr"/>
@@ -7260,15 +7264,42 @@
       <c r="F216" s="2" t="inlineStr"/>
       <c r="G216" s="2" t="inlineStr">
         <is>
+          <t>Does the proposal include separate recycling arrangements</t>
+        </is>
+      </c>
+      <c r="H216" s="2" t="inlineStr">
+        <is>
+          <t>boolean</t>
+        </is>
+      </c>
+      <c r="I216" s="2" t="inlineStr">
+        <is>
+          <t>MUST</t>
+        </is>
+      </c>
+    </row>
+    <row r="217">
+      <c r="A217" s="2" t="n"/>
+      <c r="B217" s="2" t="n"/>
+      <c r="C217" s="2" t="inlineStr">
+        <is>
+          <t>Separate recycling arrangements details</t>
+        </is>
+      </c>
+      <c r="D217" s="2" t="inlineStr"/>
+      <c r="E217" s="2" t="inlineStr"/>
+      <c r="F217" s="2" t="inlineStr"/>
+      <c r="G217" s="2" t="inlineStr">
+        <is>
           <t>Details of the recycling arrangements including types of materials, collection methods and storage facilities</t>
         </is>
       </c>
-      <c r="H216" s="2" t="inlineStr">
-        <is>
-          <t>string</t>
-        </is>
-      </c>
-      <c r="I216" s="2" t="inlineStr">
+      <c r="H217" s="2" t="inlineStr">
+        <is>
+          <t>string</t>
+        </is>
+      </c>
+      <c r="I217" s="2" t="inlineStr">
         <is>
           <t>MAY</t>
         </is>
@@ -7276,66 +7307,66 @@
     </row>
   </sheetData>
   <mergeCells count="62">
-    <mergeCell ref="A149:A153"/>
-    <mergeCell ref="A189:A197"/>
+    <mergeCell ref="B135:B149"/>
+    <mergeCell ref="B123:B134"/>
     <mergeCell ref="A92:A97"/>
     <mergeCell ref="B68"/>
-    <mergeCell ref="A187:A188"/>
-    <mergeCell ref="A164:A170"/>
+    <mergeCell ref="B214:B217"/>
     <mergeCell ref="A72:A74"/>
-    <mergeCell ref="B134:B148"/>
-    <mergeCell ref="A208:A212"/>
     <mergeCell ref="B32:B39"/>
     <mergeCell ref="A68"/>
-    <mergeCell ref="B154:B163"/>
+    <mergeCell ref="A150:A154"/>
+    <mergeCell ref="A155:A164"/>
+    <mergeCell ref="B199:B204"/>
     <mergeCell ref="A21:A27"/>
     <mergeCell ref="B102:B107"/>
-    <mergeCell ref="B171:B186"/>
     <mergeCell ref="B98:B101"/>
+    <mergeCell ref="A209:A213"/>
+    <mergeCell ref="A205:A206"/>
+    <mergeCell ref="A123:A134"/>
+    <mergeCell ref="B172:B187"/>
+    <mergeCell ref="A214:A217"/>
+    <mergeCell ref="A165:A171"/>
     <mergeCell ref="B108:B114"/>
     <mergeCell ref="A82:A91"/>
-    <mergeCell ref="B187:B188"/>
-    <mergeCell ref="B164:B170"/>
-    <mergeCell ref="A204:A205"/>
     <mergeCell ref="B115:B122"/>
     <mergeCell ref="B2:B20"/>
+    <mergeCell ref="A190:A198"/>
     <mergeCell ref="B50:B52"/>
     <mergeCell ref="A98:A101"/>
+    <mergeCell ref="B155:B164"/>
     <mergeCell ref="B28:B31"/>
-    <mergeCell ref="A171:A186"/>
-    <mergeCell ref="A213:A216"/>
-    <mergeCell ref="B189:B197"/>
-    <mergeCell ref="A198:A203"/>
+    <mergeCell ref="A188:A189"/>
     <mergeCell ref="B53:B67"/>
     <mergeCell ref="B40:B43"/>
     <mergeCell ref="B75:B81"/>
     <mergeCell ref="B44:B49"/>
-    <mergeCell ref="A206:A207"/>
+    <mergeCell ref="B205:B206"/>
+    <mergeCell ref="B207:B208"/>
+    <mergeCell ref="A135:A149"/>
     <mergeCell ref="B72:B74"/>
+    <mergeCell ref="B209:B213"/>
     <mergeCell ref="A69:A71"/>
     <mergeCell ref="B82:B91"/>
-    <mergeCell ref="B206:B207"/>
-    <mergeCell ref="B123:B133"/>
-    <mergeCell ref="A134:A148"/>
-    <mergeCell ref="B204:B205"/>
-    <mergeCell ref="B208:B212"/>
+    <mergeCell ref="B150:B154"/>
+    <mergeCell ref="B165:B171"/>
     <mergeCell ref="A50:A52"/>
     <mergeCell ref="B21:B27"/>
-    <mergeCell ref="B149:B153"/>
+    <mergeCell ref="A172:A187"/>
+    <mergeCell ref="B190:B198"/>
     <mergeCell ref="A108:A114"/>
     <mergeCell ref="A32:A39"/>
     <mergeCell ref="A115:A122"/>
     <mergeCell ref="A53:A67"/>
-    <mergeCell ref="A123:A133"/>
+    <mergeCell ref="B188:B189"/>
     <mergeCell ref="B92:B97"/>
     <mergeCell ref="A2:A20"/>
-    <mergeCell ref="A154:A163"/>
-    <mergeCell ref="B198:B203"/>
     <mergeCell ref="A28:A31"/>
-    <mergeCell ref="B213:B216"/>
     <mergeCell ref="B69:B71"/>
+    <mergeCell ref="A199:A204"/>
     <mergeCell ref="A44:A49"/>
     <mergeCell ref="A102:A107"/>
+    <mergeCell ref="A207:A208"/>
     <mergeCell ref="A40:A43"/>
     <mergeCell ref="A75:A81"/>
   </mergeCells>

</xml_diff>